<commit_message>
Notas 8 pm 12 jun
</commit_message>
<xml_diff>
--- a/Notas/Notas Monitoria.xlsx
+++ b/Notas/Notas Monitoria.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alejandro\Desktop\Monitorias\Notas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B745F6A-FAF7-4920-BFA1-926CC9B07098}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1C8BE54-4CB0-4F4C-9A0D-88071B276A3E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="83">
   <si>
     <t>BUENO MONTOYA CARLOS ANDRES</t>
   </si>
@@ -271,6 +271,9 @@
   </si>
   <si>
     <t>4.2</t>
+  </si>
+  <si>
+    <t>3.8</t>
   </si>
 </sst>
 </file>
@@ -494,7 +497,27 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="34">
+  <dxfs count="89">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -507,6 +530,441 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -685,6 +1143,31 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -705,6 +1188,41 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C5700"/>
       </font>
       <fill>
@@ -715,6 +1233,36 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -795,31 +1343,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -900,13 +1423,13 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5E3ACDE8-A7C1-4D36-97E4-0F24A76B8D04}" name="Tabla1" displayName="Tabla1" ref="A3:G71" totalsRowShown="0">
   <autoFilter ref="A3:G71" xr:uid="{DAC72CA5-81A2-4CC0-9820-08D51196F315}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{5B7101A1-8911-420E-B200-01BADAC2ABE6}" name=" " dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{58B896E8-BC7D-43FC-929C-700FF7F57F05}" name="Nombre Estudiante" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{3A1E37B4-BFB3-4620-8FBD-F7BFE149CDBA}" name="Nota 1" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{EC1EC678-EF45-47F2-BF14-25B6DC73FB40}" name="Nota 2" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{95159755-7D6F-4C5C-B09E-A60C627C7D39}" name="Nota" dataDxfId="6"/>
-    <tableColumn id="6" xr3:uid="{4F043079-D370-4D8E-AADA-1FF0019F1173}" name="Nota " dataDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{F3298C1A-32CA-46FD-ADBE-27564A2E9862}" name="Nota 3" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{5B7101A1-8911-420E-B200-01BADAC2ABE6}" name=" " dataDxfId="58"/>
+    <tableColumn id="2" xr3:uid="{58B896E8-BC7D-43FC-929C-700FF7F57F05}" name="Nombre Estudiante" dataDxfId="57"/>
+    <tableColumn id="3" xr3:uid="{3A1E37B4-BFB3-4620-8FBD-F7BFE149CDBA}" name="Nota 1" dataDxfId="56"/>
+    <tableColumn id="4" xr3:uid="{EC1EC678-EF45-47F2-BF14-25B6DC73FB40}" name="Nota 2" dataDxfId="55"/>
+    <tableColumn id="5" xr3:uid="{95159755-7D6F-4C5C-B09E-A60C627C7D39}" name="Nota" dataDxfId="54"/>
+    <tableColumn id="6" xr3:uid="{4F043079-D370-4D8E-AADA-1FF0019F1173}" name="Nota " dataDxfId="53"/>
+    <tableColumn id="7" xr3:uid="{F3298C1A-32CA-46FD-ADBE-27564A2E9862}" name="Nota 3" dataDxfId="52"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1177,8 +1700,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="G63" sqref="G63"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="G62" sqref="G62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1265,8 +1788,12 @@
       <c r="E5" s="5">
         <v>0</v>
       </c>
-      <c r="F5" s="9"/>
-      <c r="G5" s="5"/>
+      <c r="F5" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
@@ -1284,7 +1811,9 @@
       <c r="E6" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="F6" s="9"/>
+      <c r="F6" s="6" t="s">
+        <v>70</v>
+      </c>
       <c r="G6" s="5"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -1401,7 +1930,9 @@
       <c r="F12" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="G12" s="5"/>
+      <c r="G12" s="10" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
@@ -1519,7 +2050,9 @@
       <c r="F18" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="G18" s="5"/>
+      <c r="G18" s="10" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
@@ -1715,7 +2248,9 @@
       <c r="F28" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="G28" s="5"/>
+      <c r="G28" s="6" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
@@ -1790,8 +2325,12 @@
       <c r="E32" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="F32" s="9"/>
-      <c r="G32" s="5"/>
+      <c r="F32" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="G32" s="6" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
@@ -1905,7 +2444,9 @@
         <v>70</v>
       </c>
       <c r="F38" s="9"/>
-      <c r="G38" s="5"/>
+      <c r="G38" s="6" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
@@ -2056,7 +2597,9 @@
       <c r="E46" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="F46" s="9"/>
+      <c r="F46" s="6" t="s">
+        <v>70</v>
+      </c>
       <c r="G46" s="5"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
@@ -2075,7 +2618,9 @@
       <c r="E47" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="F47" s="9"/>
+      <c r="F47" s="6" t="s">
+        <v>70</v>
+      </c>
       <c r="G47" s="5"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
@@ -2151,7 +2696,9 @@
       <c r="E51" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="F51" s="9"/>
+      <c r="F51" s="6" t="s">
+        <v>70</v>
+      </c>
       <c r="G51" s="5"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
@@ -2227,7 +2774,9 @@
       <c r="E55" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="F55" s="9"/>
+      <c r="F55" s="6" t="s">
+        <v>70</v>
+      </c>
       <c r="G55" s="5"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
@@ -2246,7 +2795,9 @@
       <c r="E56" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="F56" s="9"/>
+      <c r="F56" s="6" t="s">
+        <v>70</v>
+      </c>
       <c r="G56" s="5"/>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
@@ -2360,7 +2911,9 @@
       <c r="E62" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="F62" s="9"/>
+      <c r="F62" s="6" t="s">
+        <v>70</v>
+      </c>
       <c r="G62" s="6" t="s">
         <v>81</v>
       </c>
@@ -2497,7 +3050,9 @@
       <c r="E69" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="F69" s="9"/>
+      <c r="F69" s="6" t="s">
+        <v>70</v>
+      </c>
       <c r="G69" s="5"/>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
@@ -2548,118 +3103,341 @@
     <mergeCell ref="C2:E2"/>
   </mergeCells>
   <conditionalFormatting sqref="E4:E71">
-    <cfRule type="cellIs" dxfId="33" priority="27" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="88" priority="80" operator="greaterThan">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="87" priority="74" operator="equal">
       <formula>"3.0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F4:F11 F13 F15:F71">
-    <cfRule type="cellIs" dxfId="31" priority="26" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="86" priority="79" operator="greaterThan">
       <formula>"3.0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F12">
-    <cfRule type="cellIs" dxfId="30" priority="25" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="85" priority="78" operator="greaterThan">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F14">
-    <cfRule type="cellIs" dxfId="29" priority="24" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="84" priority="77" operator="greaterThan">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4:F71">
-    <cfRule type="cellIs" dxfId="28" priority="23" operator="between">
+    <cfRule type="cellIs" dxfId="8" priority="76" operator="between">
       <formula>3</formula>
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="22" operator="between">
+    <cfRule type="cellIs" dxfId="7" priority="75" operator="between">
       <formula>"2.9"</formula>
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="73" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F18">
-    <cfRule type="cellIs" dxfId="25" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="71" operator="equal">
       <formula>"3.0"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="19" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="82" priority="72" operator="greaterThan">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F8">
-    <cfRule type="cellIs" dxfId="23" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="69" operator="equal">
       <formula>"3.0"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="17" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="80" priority="70" operator="greaterThan">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F66">
-    <cfRule type="cellIs" dxfId="21" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="67" operator="equal">
       <formula>"3.0"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="15" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="78" priority="68" operator="greaterThan">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G62">
-    <cfRule type="cellIs" dxfId="19" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="63" operator="equal">
       <formula>"3.0"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="13" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="76" priority="66" operator="greaterThan">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G62">
-    <cfRule type="cellIs" dxfId="17" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="62" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="11" operator="between">
+    <cfRule type="cellIs" dxfId="74" priority="64" operator="between">
       <formula>"2.9"</formula>
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="12" operator="between">
+    <cfRule type="cellIs" dxfId="73" priority="65" operator="between">
       <formula>3</formula>
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F28">
-    <cfRule type="cellIs" dxfId="14" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="60" operator="equal">
       <formula>"3.0"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="71" priority="61" operator="greaterThan">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F70">
-    <cfRule type="cellIs" dxfId="12" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="58" operator="equal">
       <formula>"3.0"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="69" priority="59" operator="greaterThan">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G21">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="68" priority="57" operator="greaterThan">
       <formula>"3.0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G21">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="54" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="66" priority="55" operator="between">
       <formula>"2.9"</formula>
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="between">
+    <cfRule type="cellIs" dxfId="65" priority="56" operator="between">
       <formula>3</formula>
       <formula>4</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G18">
+    <cfRule type="cellIs" dxfId="64" priority="53" operator="greaterThan">
+      <formula>"3.0"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G18">
+    <cfRule type="cellIs" dxfId="63" priority="50" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="62" priority="51" operator="between">
+      <formula>"2.9"</formula>
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="61" priority="52" operator="between">
+      <formula>3</formula>
+      <formula>4</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G18">
+    <cfRule type="cellIs" dxfId="60" priority="48" operator="equal">
+      <formula>"3.0"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="59" priority="49" operator="greaterThan">
+      <formula>3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F51">
+    <cfRule type="cellIs" dxfId="50" priority="46" operator="equal">
+      <formula>"3.0"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="51" priority="47" operator="greaterThan">
+      <formula>3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F69">
+    <cfRule type="cellIs" dxfId="48" priority="44" operator="equal">
+      <formula>"3.0"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="49" priority="45" operator="greaterThan">
+      <formula>3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F55">
+    <cfRule type="cellIs" dxfId="46" priority="42" operator="equal">
+      <formula>"3.0"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="47" priority="43" operator="greaterThan">
+      <formula>3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F5">
+    <cfRule type="cellIs" dxfId="44" priority="40" operator="equal">
+      <formula>"3.0"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="45" priority="41" operator="greaterThan">
+      <formula>3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F32">
+    <cfRule type="cellIs" dxfId="42" priority="38" operator="equal">
+      <formula>"3.0"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="43" priority="39" operator="greaterThan">
+      <formula>3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F6">
+    <cfRule type="cellIs" dxfId="40" priority="36" operator="equal">
+      <formula>"3.0"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="41" priority="37" operator="greaterThan">
+      <formula>3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G5">
+    <cfRule type="cellIs" dxfId="39" priority="35" operator="greaterThan">
+      <formula>"3.0"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G5">
+    <cfRule type="cellIs" dxfId="36" priority="32" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="37" priority="33" operator="between">
+      <formula>"2.9"</formula>
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="38" priority="34" operator="between">
+      <formula>3</formula>
+      <formula>4</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G5">
+    <cfRule type="cellIs" dxfId="35" priority="30" operator="equal">
+      <formula>"3.0"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="34" priority="31" operator="greaterThan">
+      <formula>3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G32">
+    <cfRule type="cellIs" dxfId="33" priority="29" operator="greaterThan">
+      <formula>"3.0"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G32">
+    <cfRule type="cellIs" dxfId="30" priority="26" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="31" priority="27" operator="between">
+      <formula>"2.9"</formula>
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="32" priority="28" operator="between">
+      <formula>3</formula>
+      <formula>4</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G32">
+    <cfRule type="cellIs" dxfId="29" priority="24" operator="equal">
+      <formula>"3.0"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="28" priority="25" operator="greaterThan">
+      <formula>3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G38">
+    <cfRule type="cellIs" dxfId="26" priority="20" operator="equal">
+      <formula>"3.0"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="27" priority="23" operator="greaterThan">
+      <formula>3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G38">
+    <cfRule type="cellIs" dxfId="23" priority="19" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="24" priority="21" operator="between">
+      <formula>"2.9"</formula>
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="25" priority="22" operator="between">
+      <formula>3</formula>
+      <formula>4</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G12">
+    <cfRule type="cellIs" dxfId="22" priority="18" operator="greaterThan">
+      <formula>3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G12">
+    <cfRule type="cellIs" dxfId="19" priority="15" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="20" priority="16" operator="between">
+      <formula>"2.9"</formula>
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="21" priority="17" operator="between">
+      <formula>3</formula>
+      <formula>4</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F56">
+    <cfRule type="cellIs" dxfId="17" priority="13" operator="equal">
+      <formula>"3.0"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="14" operator="greaterThan">
+      <formula>3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F46">
+    <cfRule type="cellIs" dxfId="15" priority="11" operator="equal">
+      <formula>"3.0"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="12" operator="greaterThan">
+      <formula>3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F47">
+    <cfRule type="cellIs" dxfId="13" priority="9" operator="equal">
+      <formula>"3.0"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="10" operator="greaterThan">
+      <formula>3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F62">
+    <cfRule type="cellIs" dxfId="11" priority="7" operator="equal">
+      <formula>"3.0"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="8" operator="greaterThan">
+      <formula>3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G28">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="greaterThan">
+      <formula>"3.0"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G28">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="between">
+      <formula>"2.9"</formula>
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="between">
+      <formula>3</formula>
+      <formula>4</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G28">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>"3.0"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThan">
+      <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Notas 9 pm 12 jun
</commit_message>
<xml_diff>
--- a/Notas/Notas Monitoria.xlsx
+++ b/Notas/Notas Monitoria.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alejandro\Desktop\Monitorias\Notas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1C8BE54-4CB0-4F4C-9A0D-88071B276A3E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71C3598D-80CB-4380-8558-28C146F44252}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="87">
   <si>
     <t>BUENO MONTOYA CARLOS ANDRES</t>
   </si>
@@ -274,6 +274,18 @@
   </si>
   <si>
     <t>3.8</t>
+  </si>
+  <si>
+    <t>3.5</t>
+  </si>
+  <si>
+    <t>4.4</t>
+  </si>
+  <si>
+    <t>4.7</t>
+  </si>
+  <si>
+    <t>4.0</t>
   </si>
 </sst>
 </file>
@@ -497,7 +509,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="89">
+  <dxfs count="134">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -555,13 +567,83 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
@@ -570,123 +652,58 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF9C0006"/>
       </font>
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
@@ -715,6 +732,46 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
     </dxf>
@@ -740,26 +797,6 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -782,11 +819,56 @@
       <font>
         <color rgb="FF9C0006"/>
       </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
@@ -815,26 +897,6 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF9C0006"/>
       </font>
     </dxf>
@@ -855,116 +917,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1178,6 +1130,86 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C5700"/>
       </font>
       <fill>
@@ -1213,46 +1245,6 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF9C5700"/>
       </font>
       <fill>
@@ -1318,31 +1310,461 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1423,13 +1845,13 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5E3ACDE8-A7C1-4D36-97E4-0F24A76B8D04}" name="Tabla1" displayName="Tabla1" ref="A3:G71" totalsRowShown="0">
   <autoFilter ref="A3:G71" xr:uid="{DAC72CA5-81A2-4CC0-9820-08D51196F315}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{5B7101A1-8911-420E-B200-01BADAC2ABE6}" name=" " dataDxfId="58"/>
-    <tableColumn id="2" xr3:uid="{58B896E8-BC7D-43FC-929C-700FF7F57F05}" name="Nombre Estudiante" dataDxfId="57"/>
-    <tableColumn id="3" xr3:uid="{3A1E37B4-BFB3-4620-8FBD-F7BFE149CDBA}" name="Nota 1" dataDxfId="56"/>
-    <tableColumn id="4" xr3:uid="{EC1EC678-EF45-47F2-BF14-25B6DC73FB40}" name="Nota 2" dataDxfId="55"/>
-    <tableColumn id="5" xr3:uid="{95159755-7D6F-4C5C-B09E-A60C627C7D39}" name="Nota" dataDxfId="54"/>
-    <tableColumn id="6" xr3:uid="{4F043079-D370-4D8E-AADA-1FF0019F1173}" name="Nota " dataDxfId="53"/>
-    <tableColumn id="7" xr3:uid="{F3298C1A-32CA-46FD-ADBE-27564A2E9862}" name="Nota 3" dataDxfId="52"/>
+    <tableColumn id="1" xr3:uid="{5B7101A1-8911-420E-B200-01BADAC2ABE6}" name=" " dataDxfId="53"/>
+    <tableColumn id="2" xr3:uid="{58B896E8-BC7D-43FC-929C-700FF7F57F05}" name="Nombre Estudiante" dataDxfId="52"/>
+    <tableColumn id="3" xr3:uid="{3A1E37B4-BFB3-4620-8FBD-F7BFE149CDBA}" name="Nota 1" dataDxfId="51"/>
+    <tableColumn id="4" xr3:uid="{EC1EC678-EF45-47F2-BF14-25B6DC73FB40}" name="Nota 2" dataDxfId="50"/>
+    <tableColumn id="5" xr3:uid="{95159755-7D6F-4C5C-B09E-A60C627C7D39}" name="Nota" dataDxfId="49"/>
+    <tableColumn id="6" xr3:uid="{4F043079-D370-4D8E-AADA-1FF0019F1173}" name="Nota " dataDxfId="48"/>
+    <tableColumn id="7" xr3:uid="{F3298C1A-32CA-46FD-ADBE-27564A2E9862}" name="Nota 3" dataDxfId="47"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1700,8 +2122,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="G62" sqref="G62"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="G59" sqref="G59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1972,7 +2394,9 @@
       <c r="F14" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="G14" s="5"/>
+      <c r="G14" s="10" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
@@ -2287,8 +2711,12 @@
       <c r="E30" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="F30" s="9"/>
-      <c r="G30" s="5"/>
+      <c r="F30" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="G30" s="7" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
@@ -2306,8 +2734,12 @@
       <c r="E31" s="5">
         <v>0</v>
       </c>
-      <c r="F31" s="9"/>
-      <c r="G31" s="5"/>
+      <c r="F31" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="G31" s="7" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
@@ -2367,8 +2799,12 @@
       <c r="E34" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="F34" s="9"/>
-      <c r="G34" s="5"/>
+      <c r="F34" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="G34" s="7" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
@@ -2798,7 +3234,9 @@
       <c r="F56" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="G56" s="5"/>
+      <c r="G56" s="6" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
@@ -2835,8 +3273,12 @@
       <c r="E58" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="F58" s="9"/>
-      <c r="G58" s="5"/>
+      <c r="F58" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="G58" s="6" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
@@ -2994,7 +3436,9 @@
       <c r="F66" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="G66" s="5"/>
+      <c r="G66" s="16" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
@@ -3012,8 +3456,12 @@
       <c r="E67" s="5">
         <v>0</v>
       </c>
-      <c r="F67" s="9"/>
-      <c r="G67" s="5"/>
+      <c r="F67" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="G67" s="10" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
@@ -3103,323 +3551,524 @@
     <mergeCell ref="C2:E2"/>
   </mergeCells>
   <conditionalFormatting sqref="E4:E71">
-    <cfRule type="cellIs" dxfId="88" priority="80" operator="greaterThan">
-      <formula>3</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="87" priority="74" operator="equal">
+    <cfRule type="cellIs" dxfId="133" priority="127" operator="greaterThan">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="132" priority="121" operator="equal">
       <formula>"3.0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F4:F11 F13 F15:F71">
-    <cfRule type="cellIs" dxfId="86" priority="79" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="131" priority="126" operator="greaterThan">
       <formula>"3.0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F12">
-    <cfRule type="cellIs" dxfId="85" priority="78" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="130" priority="125" operator="greaterThan">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F14">
-    <cfRule type="cellIs" dxfId="84" priority="77" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="129" priority="124" operator="greaterThan">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4:F71">
-    <cfRule type="cellIs" dxfId="8" priority="76" operator="between">
+    <cfRule type="cellIs" dxfId="128" priority="123" operator="between">
       <formula>3</formula>
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="75" operator="between">
+    <cfRule type="cellIs" dxfId="127" priority="122" operator="between">
       <formula>"2.9"</formula>
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="73" operator="equal">
+    <cfRule type="cellIs" dxfId="126" priority="120" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F18">
-    <cfRule type="cellIs" dxfId="83" priority="71" operator="equal">
+    <cfRule type="cellIs" dxfId="125" priority="118" operator="equal">
       <formula>"3.0"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="82" priority="72" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="124" priority="119" operator="greaterThan">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F8">
-    <cfRule type="cellIs" dxfId="81" priority="69" operator="equal">
+    <cfRule type="cellIs" dxfId="123" priority="116" operator="equal">
       <formula>"3.0"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="80" priority="70" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="122" priority="117" operator="greaterThan">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F66">
-    <cfRule type="cellIs" dxfId="79" priority="67" operator="equal">
+    <cfRule type="cellIs" dxfId="121" priority="114" operator="equal">
       <formula>"3.0"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="78" priority="68" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="120" priority="115" operator="greaterThan">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G62">
-    <cfRule type="cellIs" dxfId="77" priority="63" operator="equal">
+    <cfRule type="cellIs" dxfId="119" priority="110" operator="equal">
       <formula>"3.0"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="76" priority="66" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="118" priority="113" operator="greaterThan">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G62">
-    <cfRule type="cellIs" dxfId="75" priority="62" operator="equal">
+    <cfRule type="cellIs" dxfId="117" priority="109" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="74" priority="64" operator="between">
+    <cfRule type="cellIs" dxfId="116" priority="111" operator="between">
       <formula>"2.9"</formula>
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="73" priority="65" operator="between">
+    <cfRule type="cellIs" dxfId="115" priority="112" operator="between">
       <formula>3</formula>
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F28">
-    <cfRule type="cellIs" dxfId="72" priority="60" operator="equal">
+    <cfRule type="cellIs" dxfId="114" priority="107" operator="equal">
       <formula>"3.0"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="71" priority="61" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="113" priority="108" operator="greaterThan">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F70">
-    <cfRule type="cellIs" dxfId="70" priority="58" operator="equal">
+    <cfRule type="cellIs" dxfId="112" priority="105" operator="equal">
       <formula>"3.0"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="69" priority="59" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="111" priority="106" operator="greaterThan">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G21">
-    <cfRule type="cellIs" dxfId="68" priority="57" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="110" priority="104" operator="greaterThan">
       <formula>"3.0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G21">
-    <cfRule type="cellIs" dxfId="67" priority="54" operator="equal">
+    <cfRule type="cellIs" dxfId="109" priority="101" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="55" operator="between">
+    <cfRule type="cellIs" dxfId="108" priority="102" operator="between">
       <formula>"2.9"</formula>
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="65" priority="56" operator="between">
+    <cfRule type="cellIs" dxfId="107" priority="103" operator="between">
       <formula>3</formula>
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G18">
-    <cfRule type="cellIs" dxfId="64" priority="53" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="106" priority="100" operator="greaterThan">
       <formula>"3.0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G18">
-    <cfRule type="cellIs" dxfId="63" priority="50" operator="equal">
+    <cfRule type="cellIs" dxfId="105" priority="97" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="51" operator="between">
+    <cfRule type="cellIs" dxfId="104" priority="98" operator="between">
       <formula>"2.9"</formula>
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="61" priority="52" operator="between">
+    <cfRule type="cellIs" dxfId="103" priority="99" operator="between">
       <formula>3</formula>
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G18">
-    <cfRule type="cellIs" dxfId="60" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="102" priority="95" operator="equal">
       <formula>"3.0"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="59" priority="49" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="101" priority="96" operator="greaterThan">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F51">
-    <cfRule type="cellIs" dxfId="50" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="100" priority="93" operator="equal">
       <formula>"3.0"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="51" priority="47" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="99" priority="94" operator="greaterThan">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F69">
-    <cfRule type="cellIs" dxfId="48" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="98" priority="91" operator="equal">
       <formula>"3.0"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="45" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="97" priority="92" operator="greaterThan">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F55">
-    <cfRule type="cellIs" dxfId="46" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="96" priority="89" operator="equal">
       <formula>"3.0"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="47" priority="43" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="95" priority="90" operator="greaterThan">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F5">
-    <cfRule type="cellIs" dxfId="44" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="94" priority="87" operator="equal">
       <formula>"3.0"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="41" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="93" priority="88" operator="greaterThan">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F32">
-    <cfRule type="cellIs" dxfId="42" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="92" priority="85" operator="equal">
       <formula>"3.0"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="39" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="91" priority="86" operator="greaterThan">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F6">
-    <cfRule type="cellIs" dxfId="40" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="90" priority="83" operator="equal">
       <formula>"3.0"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="37" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="89" priority="84" operator="greaterThan">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5">
-    <cfRule type="cellIs" dxfId="39" priority="35" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="88" priority="82" operator="greaterThan">
       <formula>"3.0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5">
-    <cfRule type="cellIs" dxfId="36" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="87" priority="79" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="33" operator="between">
+    <cfRule type="cellIs" dxfId="86" priority="80" operator="between">
       <formula>"2.9"</formula>
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="34" operator="between">
+    <cfRule type="cellIs" dxfId="85" priority="81" operator="between">
       <formula>3</formula>
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5">
-    <cfRule type="cellIs" dxfId="35" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="77" operator="equal">
       <formula>"3.0"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="31" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="83" priority="78" operator="greaterThan">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G32">
-    <cfRule type="cellIs" dxfId="33" priority="29" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="82" priority="76" operator="greaterThan">
       <formula>"3.0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G32">
-    <cfRule type="cellIs" dxfId="30" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="73" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="27" operator="between">
+    <cfRule type="cellIs" dxfId="80" priority="74" operator="between">
       <formula>"2.9"</formula>
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="28" operator="between">
+    <cfRule type="cellIs" dxfId="79" priority="75" operator="between">
       <formula>3</formula>
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G32">
-    <cfRule type="cellIs" dxfId="29" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="71" operator="equal">
       <formula>"3.0"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="25" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="77" priority="72" operator="greaterThan">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G38">
-    <cfRule type="cellIs" dxfId="26" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="67" operator="equal">
       <formula>"3.0"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="23" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="75" priority="70" operator="greaterThan">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G38">
-    <cfRule type="cellIs" dxfId="23" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="66" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="21" operator="between">
+    <cfRule type="cellIs" dxfId="73" priority="68" operator="between">
       <formula>"2.9"</formula>
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="22" operator="between">
+    <cfRule type="cellIs" dxfId="72" priority="69" operator="between">
       <formula>3</formula>
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G12">
-    <cfRule type="cellIs" dxfId="22" priority="18" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="71" priority="65" operator="greaterThan">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G12">
-    <cfRule type="cellIs" dxfId="19" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="62" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="16" operator="between">
+    <cfRule type="cellIs" dxfId="69" priority="63" operator="between">
       <formula>"2.9"</formula>
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="17" operator="between">
+    <cfRule type="cellIs" dxfId="68" priority="64" operator="between">
       <formula>3</formula>
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F56">
-    <cfRule type="cellIs" dxfId="17" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="60" operator="equal">
       <formula>"3.0"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="14" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="66" priority="61" operator="greaterThan">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F46">
-    <cfRule type="cellIs" dxfId="15" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="58" operator="equal">
       <formula>"3.0"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="12" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="64" priority="59" operator="greaterThan">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F47">
-    <cfRule type="cellIs" dxfId="13" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="56" operator="equal">
       <formula>"3.0"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="10" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="62" priority="57" operator="greaterThan">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F62">
-    <cfRule type="cellIs" dxfId="11" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="54" operator="equal">
       <formula>"3.0"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="60" priority="55" operator="greaterThan">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G28">
+    <cfRule type="cellIs" dxfId="59" priority="53" operator="greaterThan">
+      <formula>"3.0"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G28">
+    <cfRule type="cellIs" dxfId="58" priority="50" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="57" priority="51" operator="between">
+      <formula>"2.9"</formula>
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="56" priority="52" operator="between">
+      <formula>3</formula>
+      <formula>4</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G28">
+    <cfRule type="cellIs" dxfId="55" priority="48" operator="equal">
+      <formula>"3.0"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="54" priority="49" operator="greaterThan">
+      <formula>3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G30">
+    <cfRule type="cellIs" dxfId="45" priority="44" operator="equal">
+      <formula>"3.0"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="46" priority="47" operator="greaterThan">
+      <formula>3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G30">
+    <cfRule type="cellIs" dxfId="42" priority="43" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="43" priority="45" operator="between">
+      <formula>"2.9"</formula>
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="44" priority="46" operator="between">
+      <formula>3</formula>
+      <formula>4</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G66">
+    <cfRule type="cellIs" dxfId="41" priority="42" operator="greaterThan">
+      <formula>"3.0"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G66">
+    <cfRule type="cellIs" dxfId="38" priority="39" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="39" priority="40" operator="between">
+      <formula>"2.9"</formula>
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="40" priority="41" operator="between">
+      <formula>3</formula>
+      <formula>4</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G66">
+    <cfRule type="cellIs" dxfId="37" priority="37" operator="equal">
+      <formula>"3.0"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="36" priority="38" operator="greaterThan">
+      <formula>3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G14">
+    <cfRule type="cellIs" dxfId="35" priority="36" operator="greaterThan">
+      <formula>3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G14">
+    <cfRule type="cellIs" dxfId="34" priority="33" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="33" priority="34" operator="between">
+      <formula>"2.9"</formula>
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="32" priority="35" operator="between">
+      <formula>3</formula>
+      <formula>4</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G56">
+    <cfRule type="cellIs" dxfId="31" priority="32" operator="greaterThan">
+      <formula>"3.0"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G56">
+    <cfRule type="cellIs" dxfId="28" priority="29" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="29" priority="30" operator="between">
+      <formula>"2.9"</formula>
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="30" priority="31" operator="between">
+      <formula>3</formula>
+      <formula>4</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G56">
+    <cfRule type="cellIs" dxfId="27" priority="27" operator="equal">
+      <formula>"3.0"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="26" priority="28" operator="greaterThan">
+      <formula>3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F67">
+    <cfRule type="cellIs" dxfId="25" priority="25" operator="equal">
+      <formula>"3.0"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="24" priority="26" operator="greaterThan">
+      <formula>3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G67">
+    <cfRule type="cellIs" dxfId="23" priority="24" operator="greaterThan">
+      <formula>"3.0"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G67">
+    <cfRule type="cellIs" dxfId="20" priority="21" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="21" priority="22" operator="between">
+      <formula>"2.9"</formula>
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="23" operator="between">
+      <formula>3</formula>
+      <formula>4</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G67">
+    <cfRule type="cellIs" dxfId="19" priority="19" operator="equal">
+      <formula>"3.0"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="20" operator="greaterThan">
+      <formula>3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G31">
+    <cfRule type="cellIs" dxfId="17" priority="15" operator="equal">
+      <formula>"3.0"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="18" operator="greaterThan">
+      <formula>3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G31">
+    <cfRule type="cellIs" dxfId="15" priority="14" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="16" operator="between">
+      <formula>"2.9"</formula>
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="13" priority="17" operator="between">
+      <formula>3</formula>
+      <formula>4</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G34">
+    <cfRule type="cellIs" dxfId="12" priority="10" operator="equal">
+      <formula>"3.0"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="11" priority="13" operator="greaterThan">
+      <formula>3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G34">
+    <cfRule type="cellIs" dxfId="10" priority="9" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="9" priority="11" operator="between">
+      <formula>"2.9"</formula>
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="12" operator="between">
+      <formula>3</formula>
+      <formula>4</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F58">
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
+      <formula>"3.0"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="greaterThan">
+      <formula>3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G58">
     <cfRule type="cellIs" dxfId="5" priority="6" operator="greaterThan">
       <formula>"3.0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G28">
+  <conditionalFormatting sqref="G58">
     <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
@@ -3432,7 +4081,7 @@
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G28">
+  <conditionalFormatting sqref="G58">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"3.0"</formula>
     </cfRule>

</xml_diff>

<commit_message>
Notas 11 pm 12 Junio
</commit_message>
<xml_diff>
--- a/Notas/Notas Monitoria.xlsx
+++ b/Notas/Notas Monitoria.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alejandro\Desktop\Monitorias\Notas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71C3598D-80CB-4380-8558-28C146F44252}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{109B83CC-16FE-4F32-B597-E9D7E28316C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="89">
   <si>
     <t>BUENO MONTOYA CARLOS ANDRES</t>
   </si>
@@ -286,6 +286,12 @@
   </si>
   <si>
     <t>4.0</t>
+  </si>
+  <si>
+    <t>4.6</t>
+  </si>
+  <si>
+    <t>4.5</t>
   </si>
 </sst>
 </file>
@@ -509,434 +515,24 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="134">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
+  <dxfs count="135">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1075,6 +671,426 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -1845,13 +1861,13 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5E3ACDE8-A7C1-4D36-97E4-0F24A76B8D04}" name="Tabla1" displayName="Tabla1" ref="A3:G71" totalsRowShown="0">
   <autoFilter ref="A3:G71" xr:uid="{DAC72CA5-81A2-4CC0-9820-08D51196F315}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{5B7101A1-8911-420E-B200-01BADAC2ABE6}" name=" " dataDxfId="53"/>
-    <tableColumn id="2" xr3:uid="{58B896E8-BC7D-43FC-929C-700FF7F57F05}" name="Nombre Estudiante" dataDxfId="52"/>
-    <tableColumn id="3" xr3:uid="{3A1E37B4-BFB3-4620-8FBD-F7BFE149CDBA}" name="Nota 1" dataDxfId="51"/>
-    <tableColumn id="4" xr3:uid="{EC1EC678-EF45-47F2-BF14-25B6DC73FB40}" name="Nota 2" dataDxfId="50"/>
-    <tableColumn id="5" xr3:uid="{95159755-7D6F-4C5C-B09E-A60C627C7D39}" name="Nota" dataDxfId="49"/>
-    <tableColumn id="6" xr3:uid="{4F043079-D370-4D8E-AADA-1FF0019F1173}" name="Nota " dataDxfId="48"/>
-    <tableColumn id="7" xr3:uid="{F3298C1A-32CA-46FD-ADBE-27564A2E9862}" name="Nota 3" dataDxfId="47"/>
+    <tableColumn id="1" xr3:uid="{5B7101A1-8911-420E-B200-01BADAC2ABE6}" name=" " dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{58B896E8-BC7D-43FC-929C-700FF7F57F05}" name="Nombre Estudiante" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{3A1E37B4-BFB3-4620-8FBD-F7BFE149CDBA}" name="Nota 1" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{EC1EC678-EF45-47F2-BF14-25B6DC73FB40}" name="Nota 2" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{95159755-7D6F-4C5C-B09E-A60C627C7D39}" name="Nota" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{4F043079-D370-4D8E-AADA-1FF0019F1173}" name="Nota " dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{F3298C1A-32CA-46FD-ADBE-27564A2E9862}" name="Nota 3" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2122,8 +2138,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="G59" sqref="G59"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="F46" sqref="F46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2712,7 +2728,7 @@
         <v>72</v>
       </c>
       <c r="F30" s="9" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="G30" s="7" t="s">
         <v>83</v>
@@ -2735,10 +2751,10 @@
         <v>0</v>
       </c>
       <c r="F31" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="G31" s="7" t="s">
-        <v>83</v>
+        <v>88</v>
+      </c>
+      <c r="G31" s="9" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -2800,7 +2816,7 @@
         <v>72</v>
       </c>
       <c r="F34" s="9" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="G34" s="7" t="s">
         <v>83</v>
@@ -3014,7 +3030,9 @@
       <c r="E45" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="F45" s="9"/>
+      <c r="F45" s="6" t="s">
+        <v>70</v>
+      </c>
       <c r="G45" s="5"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
@@ -3277,7 +3295,7 @@
         <v>70</v>
       </c>
       <c r="G58" s="6" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
@@ -3551,537 +3569,542 @@
     <mergeCell ref="C2:E2"/>
   </mergeCells>
   <conditionalFormatting sqref="E4:E71">
-    <cfRule type="cellIs" dxfId="133" priority="127" operator="greaterThan">
-      <formula>3</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="132" priority="121" operator="equal">
+    <cfRule type="cellIs" dxfId="134" priority="133" operator="greaterThan">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="133" priority="127" operator="equal">
       <formula>"3.0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F4:F11 F13 F15:F71">
-    <cfRule type="cellIs" dxfId="131" priority="126" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="132" priority="132" operator="greaterThan">
       <formula>"3.0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F12">
-    <cfRule type="cellIs" dxfId="130" priority="125" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="131" priority="131" operator="greaterThan">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F14">
-    <cfRule type="cellIs" dxfId="129" priority="124" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="130" priority="130" operator="greaterThan">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4:F71">
-    <cfRule type="cellIs" dxfId="128" priority="123" operator="between">
+    <cfRule type="cellIs" dxfId="129" priority="129" operator="between">
       <formula>3</formula>
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="127" priority="122" operator="between">
+    <cfRule type="cellIs" dxfId="128" priority="128" operator="between">
       <formula>"2.9"</formula>
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="126" priority="120" operator="equal">
+    <cfRule type="cellIs" dxfId="127" priority="126" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F18">
-    <cfRule type="cellIs" dxfId="125" priority="118" operator="equal">
+    <cfRule type="cellIs" dxfId="126" priority="124" operator="equal">
       <formula>"3.0"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="124" priority="119" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="125" priority="125" operator="greaterThan">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F8">
-    <cfRule type="cellIs" dxfId="123" priority="116" operator="equal">
+    <cfRule type="cellIs" dxfId="124" priority="122" operator="equal">
       <formula>"3.0"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="122" priority="117" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="123" priority="123" operator="greaterThan">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F66">
-    <cfRule type="cellIs" dxfId="121" priority="114" operator="equal">
+    <cfRule type="cellIs" dxfId="122" priority="120" operator="equal">
       <formula>"3.0"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="120" priority="115" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="121" priority="121" operator="greaterThan">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G62">
-    <cfRule type="cellIs" dxfId="119" priority="110" operator="equal">
+    <cfRule type="cellIs" dxfId="120" priority="116" operator="equal">
       <formula>"3.0"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="118" priority="113" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="119" priority="119" operator="greaterThan">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G62">
-    <cfRule type="cellIs" dxfId="117" priority="109" operator="equal">
+    <cfRule type="cellIs" dxfId="118" priority="115" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="116" priority="111" operator="between">
+    <cfRule type="cellIs" dxfId="117" priority="117" operator="between">
       <formula>"2.9"</formula>
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="115" priority="112" operator="between">
+    <cfRule type="cellIs" dxfId="116" priority="118" operator="between">
       <formula>3</formula>
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F28">
-    <cfRule type="cellIs" dxfId="114" priority="107" operator="equal">
+    <cfRule type="cellIs" dxfId="115" priority="113" operator="equal">
       <formula>"3.0"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="113" priority="108" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="114" priority="114" operator="greaterThan">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F70">
-    <cfRule type="cellIs" dxfId="112" priority="105" operator="equal">
+    <cfRule type="cellIs" dxfId="113" priority="111" operator="equal">
       <formula>"3.0"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="111" priority="106" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="112" priority="112" operator="greaterThan">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G21">
-    <cfRule type="cellIs" dxfId="110" priority="104" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="111" priority="110" operator="greaterThan">
       <formula>"3.0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G21">
-    <cfRule type="cellIs" dxfId="109" priority="101" operator="equal">
+    <cfRule type="cellIs" dxfId="110" priority="107" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="108" priority="102" operator="between">
+    <cfRule type="cellIs" dxfId="109" priority="108" operator="between">
       <formula>"2.9"</formula>
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="107" priority="103" operator="between">
+    <cfRule type="cellIs" dxfId="108" priority="109" operator="between">
       <formula>3</formula>
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G18">
-    <cfRule type="cellIs" dxfId="106" priority="100" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="107" priority="106" operator="greaterThan">
       <formula>"3.0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G18">
-    <cfRule type="cellIs" dxfId="105" priority="97" operator="equal">
+    <cfRule type="cellIs" dxfId="106" priority="103" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="104" priority="98" operator="between">
+    <cfRule type="cellIs" dxfId="105" priority="104" operator="between">
       <formula>"2.9"</formula>
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="103" priority="99" operator="between">
+    <cfRule type="cellIs" dxfId="104" priority="105" operator="between">
       <formula>3</formula>
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G18">
-    <cfRule type="cellIs" dxfId="102" priority="95" operator="equal">
+    <cfRule type="cellIs" dxfId="103" priority="101" operator="equal">
       <formula>"3.0"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="101" priority="96" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="102" priority="102" operator="greaterThan">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F51">
-    <cfRule type="cellIs" dxfId="100" priority="93" operator="equal">
+    <cfRule type="cellIs" dxfId="101" priority="99" operator="equal">
       <formula>"3.0"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="99" priority="94" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="100" priority="100" operator="greaterThan">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F69">
-    <cfRule type="cellIs" dxfId="98" priority="91" operator="equal">
+    <cfRule type="cellIs" dxfId="99" priority="97" operator="equal">
       <formula>"3.0"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="97" priority="92" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="98" priority="98" operator="greaterThan">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F55">
-    <cfRule type="cellIs" dxfId="96" priority="89" operator="equal">
+    <cfRule type="cellIs" dxfId="97" priority="95" operator="equal">
       <formula>"3.0"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="95" priority="90" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="96" priority="96" operator="greaterThan">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F5">
-    <cfRule type="cellIs" dxfId="94" priority="87" operator="equal">
+    <cfRule type="cellIs" dxfId="95" priority="93" operator="equal">
       <formula>"3.0"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="93" priority="88" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="94" priority="94" operator="greaterThan">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F32">
-    <cfRule type="cellIs" dxfId="92" priority="85" operator="equal">
+    <cfRule type="cellIs" dxfId="93" priority="91" operator="equal">
       <formula>"3.0"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="91" priority="86" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="92" priority="92" operator="greaterThan">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F6">
-    <cfRule type="cellIs" dxfId="90" priority="83" operator="equal">
+    <cfRule type="cellIs" dxfId="91" priority="89" operator="equal">
       <formula>"3.0"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="89" priority="84" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="90" priority="90" operator="greaterThan">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5">
-    <cfRule type="cellIs" dxfId="88" priority="82" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="89" priority="88" operator="greaterThan">
       <formula>"3.0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5">
-    <cfRule type="cellIs" dxfId="87" priority="79" operator="equal">
+    <cfRule type="cellIs" dxfId="88" priority="85" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="86" priority="80" operator="between">
+    <cfRule type="cellIs" dxfId="87" priority="86" operator="between">
       <formula>"2.9"</formula>
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="85" priority="81" operator="between">
+    <cfRule type="cellIs" dxfId="86" priority="87" operator="between">
       <formula>3</formula>
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5">
-    <cfRule type="cellIs" dxfId="84" priority="77" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="83" operator="equal">
       <formula>"3.0"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="83" priority="78" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="84" priority="84" operator="greaterThan">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G32">
-    <cfRule type="cellIs" dxfId="82" priority="76" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="83" priority="82" operator="greaterThan">
       <formula>"3.0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G32">
-    <cfRule type="cellIs" dxfId="81" priority="73" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="79" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="80" priority="74" operator="between">
+    <cfRule type="cellIs" dxfId="81" priority="80" operator="between">
       <formula>"2.9"</formula>
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="79" priority="75" operator="between">
+    <cfRule type="cellIs" dxfId="80" priority="81" operator="between">
       <formula>3</formula>
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G32">
-    <cfRule type="cellIs" dxfId="78" priority="71" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="77" operator="equal">
       <formula>"3.0"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="77" priority="72" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="78" priority="78" operator="greaterThan">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G38">
-    <cfRule type="cellIs" dxfId="76" priority="67" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="73" operator="equal">
       <formula>"3.0"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="75" priority="70" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="76" priority="76" operator="greaterThan">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G38">
-    <cfRule type="cellIs" dxfId="74" priority="66" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="72" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="73" priority="68" operator="between">
+    <cfRule type="cellIs" dxfId="74" priority="74" operator="between">
       <formula>"2.9"</formula>
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="72" priority="69" operator="between">
+    <cfRule type="cellIs" dxfId="73" priority="75" operator="between">
       <formula>3</formula>
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G12">
-    <cfRule type="cellIs" dxfId="71" priority="65" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="72" priority="71" operator="greaterThan">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G12">
-    <cfRule type="cellIs" dxfId="70" priority="62" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="68" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="69" priority="63" operator="between">
+    <cfRule type="cellIs" dxfId="70" priority="69" operator="between">
       <formula>"2.9"</formula>
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="68" priority="64" operator="between">
+    <cfRule type="cellIs" dxfId="69" priority="70" operator="between">
       <formula>3</formula>
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F56">
-    <cfRule type="cellIs" dxfId="67" priority="60" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="66" operator="equal">
       <formula>"3.0"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="61" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="67" priority="67" operator="greaterThan">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F46">
-    <cfRule type="cellIs" dxfId="65" priority="58" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="64" operator="equal">
       <formula>"3.0"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="59" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="65" priority="65" operator="greaterThan">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F47">
-    <cfRule type="cellIs" dxfId="63" priority="56" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="62" operator="equal">
       <formula>"3.0"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="57" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="63" priority="63" operator="greaterThan">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F62">
-    <cfRule type="cellIs" dxfId="61" priority="54" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="60" operator="equal">
       <formula>"3.0"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="55" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="61" priority="61" operator="greaterThan">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G28">
-    <cfRule type="cellIs" dxfId="59" priority="53" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="60" priority="59" operator="greaterThan">
       <formula>"3.0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G28">
-    <cfRule type="cellIs" dxfId="58" priority="50" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="56" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="57" priority="51" operator="between">
+    <cfRule type="cellIs" dxfId="58" priority="57" operator="between">
       <formula>"2.9"</formula>
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="52" operator="between">
+    <cfRule type="cellIs" dxfId="57" priority="58" operator="between">
       <formula>3</formula>
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G28">
-    <cfRule type="cellIs" dxfId="55" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="54" operator="equal">
       <formula>"3.0"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="49" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="55" priority="55" operator="greaterThan">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G30">
-    <cfRule type="cellIs" dxfId="45" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="50" operator="equal">
       <formula>"3.0"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="47" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="53" priority="53" operator="greaterThan">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G30">
-    <cfRule type="cellIs" dxfId="42" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="49" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="45" operator="between">
+    <cfRule type="cellIs" dxfId="51" priority="51" operator="between">
       <formula>"2.9"</formula>
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="46" operator="between">
+    <cfRule type="cellIs" dxfId="50" priority="52" operator="between">
       <formula>3</formula>
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G66">
-    <cfRule type="cellIs" dxfId="41" priority="42" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="49" priority="48" operator="greaterThan">
       <formula>"3.0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G66">
-    <cfRule type="cellIs" dxfId="38" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="45" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="40" operator="between">
+    <cfRule type="cellIs" dxfId="47" priority="46" operator="between">
       <formula>"2.9"</formula>
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="41" operator="between">
+    <cfRule type="cellIs" dxfId="46" priority="47" operator="between">
       <formula>3</formula>
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G66">
-    <cfRule type="cellIs" dxfId="37" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="43" operator="equal">
       <formula>"3.0"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="38" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="44" priority="44" operator="greaterThan">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G14">
-    <cfRule type="cellIs" dxfId="35" priority="36" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="43" priority="42" operator="greaterThan">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G14">
-    <cfRule type="cellIs" dxfId="34" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="39" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="34" operator="between">
+    <cfRule type="cellIs" dxfId="41" priority="40" operator="between">
       <formula>"2.9"</formula>
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="35" operator="between">
+    <cfRule type="cellIs" dxfId="40" priority="41" operator="between">
       <formula>3</formula>
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G56">
-    <cfRule type="cellIs" dxfId="31" priority="32" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="39" priority="38" operator="greaterThan">
       <formula>"3.0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G56">
-    <cfRule type="cellIs" dxfId="28" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="35" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="30" operator="between">
+    <cfRule type="cellIs" dxfId="37" priority="36" operator="between">
       <formula>"2.9"</formula>
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="31" operator="between">
+    <cfRule type="cellIs" dxfId="36" priority="37" operator="between">
       <formula>3</formula>
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G56">
-    <cfRule type="cellIs" dxfId="27" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="33" operator="equal">
       <formula>"3.0"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="28" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="34" priority="34" operator="greaterThan">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F67">
-    <cfRule type="cellIs" dxfId="25" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="31" operator="equal">
       <formula>"3.0"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="26" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="32" priority="32" operator="greaterThan">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G67">
-    <cfRule type="cellIs" dxfId="23" priority="24" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="31" priority="30" operator="greaterThan">
       <formula>"3.0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G67">
-    <cfRule type="cellIs" dxfId="20" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="27" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="22" operator="between">
+    <cfRule type="cellIs" dxfId="29" priority="28" operator="between">
       <formula>"2.9"</formula>
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="23" operator="between">
+    <cfRule type="cellIs" dxfId="28" priority="29" operator="between">
       <formula>3</formula>
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G67">
-    <cfRule type="cellIs" dxfId="19" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="25" operator="equal">
       <formula>"3.0"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="20" operator="greaterThan">
-      <formula>3</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G31">
-    <cfRule type="cellIs" dxfId="17" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="26" operator="greaterThan">
+      <formula>3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G34">
+    <cfRule type="cellIs" dxfId="25" priority="16" operator="equal">
       <formula>"3.0"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="18" operator="greaterThan">
-      <formula>3</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G31">
-    <cfRule type="cellIs" dxfId="15" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="19" operator="greaterThan">
+      <formula>3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G34">
+    <cfRule type="cellIs" dxfId="23" priority="15" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="16" operator="between">
+    <cfRule type="cellIs" dxfId="22" priority="17" operator="between">
       <formula>"2.9"</formula>
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="17" operator="between">
+    <cfRule type="cellIs" dxfId="21" priority="18" operator="between">
       <formula>3</formula>
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G34">
-    <cfRule type="cellIs" dxfId="12" priority="10" operator="equal">
+  <conditionalFormatting sqref="F58">
+    <cfRule type="cellIs" dxfId="20" priority="13" operator="equal">
       <formula>"3.0"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="13" operator="greaterThan">
-      <formula>3</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G34">
-    <cfRule type="cellIs" dxfId="10" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="14" operator="greaterThan">
+      <formula>3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G58">
+    <cfRule type="cellIs" dxfId="18" priority="12" operator="greaterThan">
+      <formula>"3.0"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G58">
+    <cfRule type="cellIs" dxfId="17" priority="9" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="11" operator="between">
+    <cfRule type="cellIs" dxfId="16" priority="10" operator="between">
       <formula>"2.9"</formula>
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="12" operator="between">
+    <cfRule type="cellIs" dxfId="15" priority="11" operator="between">
       <formula>3</formula>
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F58">
-    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
+  <conditionalFormatting sqref="G58">
+    <cfRule type="cellIs" dxfId="14" priority="7" operator="equal">
       <formula>"3.0"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="8" operator="greaterThan">
-      <formula>3</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G58">
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="13" priority="8" operator="greaterThan">
+      <formula>3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G31">
+    <cfRule type="cellIs" dxfId="12" priority="6" operator="greaterThan">
       <formula>"3.0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G58">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+  <conditionalFormatting sqref="G31">
+    <cfRule type="cellIs" dxfId="11" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="between">
+    <cfRule type="cellIs" dxfId="10" priority="4" operator="between">
       <formula>"2.9"</formula>
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="between">
+    <cfRule type="cellIs" dxfId="9" priority="5" operator="between">
       <formula>3</formula>
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G58">
+  <conditionalFormatting sqref="F45">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"3.0"</formula>
     </cfRule>

</xml_diff>

<commit_message>
Clase 13 de junio mañana
</commit_message>
<xml_diff>
--- a/Notas/Notas Monitoria.xlsx
+++ b/Notas/Notas Monitoria.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alejandro\Desktop\Monitorias\Notas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{109B83CC-16FE-4F32-B597-E9D7E28316C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{819EFD44-2BD1-4C0D-8AC6-C77745E3FA30}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="91">
   <si>
     <t>BUENO MONTOYA CARLOS ANDRES</t>
   </si>
@@ -292,13 +292,19 @@
   </si>
   <si>
     <t>4.5</t>
+  </si>
+  <si>
+    <t>4.75</t>
+  </si>
+  <si>
+    <t>Pendiente</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -314,8 +320,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -331,6 +344,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -459,7 +478,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -511,28 +530,176 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="135">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
+  <dxfs count="153">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -671,6 +838,26 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C5700"/>
       </font>
       <fill>
@@ -1861,13 +2048,13 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5E3ACDE8-A7C1-4D36-97E4-0F24A76B8D04}" name="Tabla1" displayName="Tabla1" ref="A3:G71" totalsRowShown="0">
   <autoFilter ref="A3:G71" xr:uid="{DAC72CA5-81A2-4CC0-9820-08D51196F315}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{5B7101A1-8911-420E-B200-01BADAC2ABE6}" name=" " dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{58B896E8-BC7D-43FC-929C-700FF7F57F05}" name="Nombre Estudiante" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{3A1E37B4-BFB3-4620-8FBD-F7BFE149CDBA}" name="Nota 1" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{EC1EC678-EF45-47F2-BF14-25B6DC73FB40}" name="Nota 2" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{95159755-7D6F-4C5C-B09E-A60C627C7D39}" name="Nota" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{4F043079-D370-4D8E-AADA-1FF0019F1173}" name="Nota " dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{F3298C1A-32CA-46FD-ADBE-27564A2E9862}" name="Nota 3" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{5B7101A1-8911-420E-B200-01BADAC2ABE6}" name=" " dataDxfId="24"/>
+    <tableColumn id="2" xr3:uid="{58B896E8-BC7D-43FC-929C-700FF7F57F05}" name="Nombre Estudiante" dataDxfId="23"/>
+    <tableColumn id="3" xr3:uid="{3A1E37B4-BFB3-4620-8FBD-F7BFE149CDBA}" name="Nota 1" dataDxfId="22"/>
+    <tableColumn id="4" xr3:uid="{EC1EC678-EF45-47F2-BF14-25B6DC73FB40}" name="Nota 2" dataDxfId="21"/>
+    <tableColumn id="5" xr3:uid="{95159755-7D6F-4C5C-B09E-A60C627C7D39}" name="Nota" dataDxfId="20"/>
+    <tableColumn id="6" xr3:uid="{4F043079-D370-4D8E-AADA-1FF0019F1173}" name="Nota " dataDxfId="19"/>
+    <tableColumn id="7" xr3:uid="{F3298C1A-32CA-46FD-ADBE-27564A2E9862}" name="Nota 3" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2138,8 +2325,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="F46" sqref="F46"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2728,7 +2915,7 @@
         <v>72</v>
       </c>
       <c r="F30" s="9" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="G30" s="7" t="s">
         <v>83</v>
@@ -2751,9 +2938,9 @@
         <v>0</v>
       </c>
       <c r="F31" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="G31" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="G31" s="5" t="s">
         <v>88</v>
       </c>
     </row>
@@ -2816,7 +3003,7 @@
         <v>72</v>
       </c>
       <c r="F34" s="9" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="G34" s="7" t="s">
         <v>83</v>
@@ -2857,8 +3044,12 @@
       <c r="E36" s="5">
         <v>0</v>
       </c>
-      <c r="F36" s="9"/>
-      <c r="G36" s="5"/>
+      <c r="F36" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="G36" s="6" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
@@ -2935,8 +3126,12 @@
       <c r="E40" s="5">
         <v>0</v>
       </c>
-      <c r="F40" s="9"/>
-      <c r="G40" s="5"/>
+      <c r="F40" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="G40" s="6" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
@@ -3454,8 +3649,8 @@
       <c r="F66" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="G66" s="16" t="s">
-        <v>72</v>
+      <c r="G66" s="10" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
@@ -3569,126 +3764,200 @@
     <mergeCell ref="C2:E2"/>
   </mergeCells>
   <conditionalFormatting sqref="E4:E71">
-    <cfRule type="cellIs" dxfId="134" priority="133" operator="greaterThan">
-      <formula>3</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="133" priority="127" operator="equal">
+    <cfRule type="cellIs" dxfId="152" priority="151" operator="greaterThan">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="151" priority="145" operator="equal">
       <formula>"3.0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F4:F11 F13 F15:F71">
-    <cfRule type="cellIs" dxfId="132" priority="132" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="150" priority="150" operator="greaterThan">
       <formula>"3.0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F12">
-    <cfRule type="cellIs" dxfId="131" priority="131" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="149" priority="149" operator="greaterThan">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F14">
-    <cfRule type="cellIs" dxfId="130" priority="130" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="148" priority="148" operator="greaterThan">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4:F71">
-    <cfRule type="cellIs" dxfId="129" priority="129" operator="between">
+    <cfRule type="cellIs" dxfId="147" priority="147" operator="between">
       <formula>3</formula>
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="128" priority="128" operator="between">
+    <cfRule type="cellIs" dxfId="146" priority="146" operator="between">
       <formula>"2.9"</formula>
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="127" priority="126" operator="equal">
+    <cfRule type="cellIs" dxfId="145" priority="144" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F18">
-    <cfRule type="cellIs" dxfId="126" priority="124" operator="equal">
-      <formula>"3.0"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="125" priority="125" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="144" priority="142" operator="equal">
+      <formula>"3.0"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="143" priority="143" operator="greaterThan">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F8">
-    <cfRule type="cellIs" dxfId="124" priority="122" operator="equal">
-      <formula>"3.0"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="123" priority="123" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="142" priority="140" operator="equal">
+      <formula>"3.0"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="141" priority="141" operator="greaterThan">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F66">
-    <cfRule type="cellIs" dxfId="122" priority="120" operator="equal">
-      <formula>"3.0"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="121" priority="121" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="140" priority="138" operator="equal">
+      <formula>"3.0"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="139" priority="139" operator="greaterThan">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G62">
-    <cfRule type="cellIs" dxfId="120" priority="116" operator="equal">
-      <formula>"3.0"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="119" priority="119" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="138" priority="134" operator="equal">
+      <formula>"3.0"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="137" priority="137" operator="greaterThan">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G62">
-    <cfRule type="cellIs" dxfId="118" priority="115" operator="equal">
+    <cfRule type="cellIs" dxfId="136" priority="133" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="117" priority="117" operator="between">
+    <cfRule type="cellIs" dxfId="135" priority="135" operator="between">
       <formula>"2.9"</formula>
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="116" priority="118" operator="between">
+    <cfRule type="cellIs" dxfId="134" priority="136" operator="between">
       <formula>3</formula>
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F28">
-    <cfRule type="cellIs" dxfId="115" priority="113" operator="equal">
-      <formula>"3.0"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="114" priority="114" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="133" priority="131" operator="equal">
+      <formula>"3.0"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="132" priority="132" operator="greaterThan">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F70">
-    <cfRule type="cellIs" dxfId="113" priority="111" operator="equal">
-      <formula>"3.0"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="112" priority="112" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="131" priority="129" operator="equal">
+      <formula>"3.0"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="130" priority="130" operator="greaterThan">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G21">
-    <cfRule type="cellIs" dxfId="111" priority="110" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="129" priority="128" operator="greaterThan">
       <formula>"3.0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G21">
-    <cfRule type="cellIs" dxfId="110" priority="107" operator="equal">
+    <cfRule type="cellIs" dxfId="128" priority="125" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="109" priority="108" operator="between">
+    <cfRule type="cellIs" dxfId="127" priority="126" operator="between">
       <formula>"2.9"</formula>
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="108" priority="109" operator="between">
+    <cfRule type="cellIs" dxfId="126" priority="127" operator="between">
       <formula>3</formula>
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G18">
+    <cfRule type="cellIs" dxfId="125" priority="124" operator="greaterThan">
+      <formula>"3.0"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G18">
+    <cfRule type="cellIs" dxfId="124" priority="121" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="123" priority="122" operator="between">
+      <formula>"2.9"</formula>
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="122" priority="123" operator="between">
+      <formula>3</formula>
+      <formula>4</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G18">
+    <cfRule type="cellIs" dxfId="121" priority="119" operator="equal">
+      <formula>"3.0"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="120" priority="120" operator="greaterThan">
+      <formula>3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F51">
+    <cfRule type="cellIs" dxfId="119" priority="117" operator="equal">
+      <formula>"3.0"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="118" priority="118" operator="greaterThan">
+      <formula>3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F69">
+    <cfRule type="cellIs" dxfId="117" priority="115" operator="equal">
+      <formula>"3.0"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="116" priority="116" operator="greaterThan">
+      <formula>3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F55">
+    <cfRule type="cellIs" dxfId="115" priority="113" operator="equal">
+      <formula>"3.0"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="114" priority="114" operator="greaterThan">
+      <formula>3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F5">
+    <cfRule type="cellIs" dxfId="113" priority="111" operator="equal">
+      <formula>"3.0"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="112" priority="112" operator="greaterThan">
+      <formula>3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F32">
+    <cfRule type="cellIs" dxfId="111" priority="109" operator="equal">
+      <formula>"3.0"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="110" priority="110" operator="greaterThan">
+      <formula>3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F6">
+    <cfRule type="cellIs" dxfId="109" priority="107" operator="equal">
+      <formula>"3.0"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="108" priority="108" operator="greaterThan">
+      <formula>3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G5">
     <cfRule type="cellIs" dxfId="107" priority="106" operator="greaterThan">
       <formula>"3.0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G18">
+  <conditionalFormatting sqref="G5">
     <cfRule type="cellIs" dxfId="106" priority="103" operator="equal">
       <formula>0</formula>
     </cfRule>
@@ -3701,7 +3970,7 @@
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G18">
+  <conditionalFormatting sqref="G5">
     <cfRule type="cellIs" dxfId="103" priority="101" operator="equal">
       <formula>"3.0"</formula>
     </cfRule>
@@ -3709,230 +3978,208 @@
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F51">
-    <cfRule type="cellIs" dxfId="101" priority="99" operator="equal">
-      <formula>"3.0"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="100" priority="100" operator="greaterThan">
-      <formula>3</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F69">
-    <cfRule type="cellIs" dxfId="99" priority="97" operator="equal">
-      <formula>"3.0"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="98" priority="98" operator="greaterThan">
-      <formula>3</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F55">
-    <cfRule type="cellIs" dxfId="97" priority="95" operator="equal">
-      <formula>"3.0"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="96" priority="96" operator="greaterThan">
-      <formula>3</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F5">
-    <cfRule type="cellIs" dxfId="95" priority="93" operator="equal">
-      <formula>"3.0"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="94" priority="94" operator="greaterThan">
-      <formula>3</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F32">
-    <cfRule type="cellIs" dxfId="93" priority="91" operator="equal">
-      <formula>"3.0"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="92" priority="92" operator="greaterThan">
-      <formula>3</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F6">
-    <cfRule type="cellIs" dxfId="91" priority="89" operator="equal">
-      <formula>"3.0"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="90" priority="90" operator="greaterThan">
-      <formula>3</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G5">
-    <cfRule type="cellIs" dxfId="89" priority="88" operator="greaterThan">
-      <formula>"3.0"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G5">
-    <cfRule type="cellIs" dxfId="88" priority="85" operator="equal">
+  <conditionalFormatting sqref="G32">
+    <cfRule type="cellIs" dxfId="101" priority="100" operator="greaterThan">
+      <formula>"3.0"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G32">
+    <cfRule type="cellIs" dxfId="100" priority="97" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="87" priority="86" operator="between">
+    <cfRule type="cellIs" dxfId="99" priority="98" operator="between">
       <formula>"2.9"</formula>
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="86" priority="87" operator="between">
+    <cfRule type="cellIs" dxfId="98" priority="99" operator="between">
       <formula>3</formula>
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G5">
-    <cfRule type="cellIs" dxfId="85" priority="83" operator="equal">
-      <formula>"3.0"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="84" priority="84" operator="greaterThan">
-      <formula>3</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="G32">
-    <cfRule type="cellIs" dxfId="83" priority="82" operator="greaterThan">
-      <formula>"3.0"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G32">
-    <cfRule type="cellIs" dxfId="82" priority="79" operator="equal">
+    <cfRule type="cellIs" dxfId="97" priority="95" operator="equal">
+      <formula>"3.0"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="96" priority="96" operator="greaterThan">
+      <formula>3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G38">
+    <cfRule type="cellIs" dxfId="95" priority="91" operator="equal">
+      <formula>"3.0"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="94" priority="94" operator="greaterThan">
+      <formula>3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G38">
+    <cfRule type="cellIs" dxfId="93" priority="90" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="81" priority="80" operator="between">
+    <cfRule type="cellIs" dxfId="92" priority="92" operator="between">
       <formula>"2.9"</formula>
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="80" priority="81" operator="between">
+    <cfRule type="cellIs" dxfId="91" priority="93" operator="between">
       <formula>3</formula>
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G32">
-    <cfRule type="cellIs" dxfId="79" priority="77" operator="equal">
-      <formula>"3.0"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="78" priority="78" operator="greaterThan">
-      <formula>3</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G38">
-    <cfRule type="cellIs" dxfId="77" priority="73" operator="equal">
-      <formula>"3.0"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="76" priority="76" operator="greaterThan">
-      <formula>3</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G38">
-    <cfRule type="cellIs" dxfId="75" priority="72" operator="equal">
+  <conditionalFormatting sqref="G12">
+    <cfRule type="cellIs" dxfId="90" priority="89" operator="greaterThan">
+      <formula>3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G12">
+    <cfRule type="cellIs" dxfId="89" priority="86" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="74" priority="74" operator="between">
+    <cfRule type="cellIs" dxfId="88" priority="87" operator="between">
       <formula>"2.9"</formula>
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="73" priority="75" operator="between">
+    <cfRule type="cellIs" dxfId="87" priority="88" operator="between">
       <formula>3</formula>
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G12">
-    <cfRule type="cellIs" dxfId="72" priority="71" operator="greaterThan">
-      <formula>3</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G12">
-    <cfRule type="cellIs" dxfId="71" priority="68" operator="equal">
+  <conditionalFormatting sqref="F56">
+    <cfRule type="cellIs" dxfId="86" priority="84" operator="equal">
+      <formula>"3.0"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="85" priority="85" operator="greaterThan">
+      <formula>3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F46">
+    <cfRule type="cellIs" dxfId="84" priority="82" operator="equal">
+      <formula>"3.0"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="83" priority="83" operator="greaterThan">
+      <formula>3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F47">
+    <cfRule type="cellIs" dxfId="82" priority="80" operator="equal">
+      <formula>"3.0"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="81" priority="81" operator="greaterThan">
+      <formula>3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F62">
+    <cfRule type="cellIs" dxfId="80" priority="78" operator="equal">
+      <formula>"3.0"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="79" priority="79" operator="greaterThan">
+      <formula>3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G28">
+    <cfRule type="cellIs" dxfId="78" priority="77" operator="greaterThan">
+      <formula>"3.0"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G28">
+    <cfRule type="cellIs" dxfId="77" priority="74" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="70" priority="69" operator="between">
+    <cfRule type="cellIs" dxfId="76" priority="75" operator="between">
       <formula>"2.9"</formula>
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="69" priority="70" operator="between">
+    <cfRule type="cellIs" dxfId="75" priority="76" operator="between">
       <formula>3</formula>
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F56">
-    <cfRule type="cellIs" dxfId="68" priority="66" operator="equal">
-      <formula>"3.0"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="67" priority="67" operator="greaterThan">
-      <formula>3</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F46">
-    <cfRule type="cellIs" dxfId="66" priority="64" operator="equal">
-      <formula>"3.0"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="65" priority="65" operator="greaterThan">
-      <formula>3</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F47">
-    <cfRule type="cellIs" dxfId="64" priority="62" operator="equal">
-      <formula>"3.0"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="63" priority="63" operator="greaterThan">
-      <formula>3</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F62">
-    <cfRule type="cellIs" dxfId="62" priority="60" operator="equal">
-      <formula>"3.0"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="61" priority="61" operator="greaterThan">
-      <formula>3</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="G28">
-    <cfRule type="cellIs" dxfId="60" priority="59" operator="greaterThan">
-      <formula>"3.0"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G28">
-    <cfRule type="cellIs" dxfId="59" priority="56" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="72" operator="equal">
+      <formula>"3.0"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="73" priority="73" operator="greaterThan">
+      <formula>3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G30">
+    <cfRule type="cellIs" dxfId="72" priority="68" operator="equal">
+      <formula>"3.0"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="71" priority="71" operator="greaterThan">
+      <formula>3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G30">
+    <cfRule type="cellIs" dxfId="70" priority="67" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="57" operator="between">
+    <cfRule type="cellIs" dxfId="69" priority="69" operator="between">
       <formula>"2.9"</formula>
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="57" priority="58" operator="between">
+    <cfRule type="cellIs" dxfId="68" priority="70" operator="between">
       <formula>3</formula>
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G28">
-    <cfRule type="cellIs" dxfId="56" priority="54" operator="equal">
-      <formula>"3.0"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="55" priority="55" operator="greaterThan">
-      <formula>3</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G30">
-    <cfRule type="cellIs" dxfId="54" priority="50" operator="equal">
-      <formula>"3.0"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="53" priority="53" operator="greaterThan">
-      <formula>3</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G30">
-    <cfRule type="cellIs" dxfId="52" priority="49" operator="equal">
+  <conditionalFormatting sqref="G14">
+    <cfRule type="cellIs" dxfId="61" priority="60" operator="greaterThan">
+      <formula>3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G14">
+    <cfRule type="cellIs" dxfId="60" priority="57" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="51" priority="51" operator="between">
+    <cfRule type="cellIs" dxfId="59" priority="58" operator="between">
       <formula>"2.9"</formula>
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="52" operator="between">
+    <cfRule type="cellIs" dxfId="58" priority="59" operator="between">
       <formula>3</formula>
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G66">
+  <conditionalFormatting sqref="G56">
+    <cfRule type="cellIs" dxfId="57" priority="56" operator="greaterThan">
+      <formula>"3.0"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G56">
+    <cfRule type="cellIs" dxfId="56" priority="53" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="55" priority="54" operator="between">
+      <formula>"2.9"</formula>
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="54" priority="55" operator="between">
+      <formula>3</formula>
+      <formula>4</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G56">
+    <cfRule type="cellIs" dxfId="53" priority="51" operator="equal">
+      <formula>"3.0"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="52" priority="52" operator="greaterThan">
+      <formula>3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F67">
+    <cfRule type="cellIs" dxfId="51" priority="49" operator="equal">
+      <formula>"3.0"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="50" priority="50" operator="greaterThan">
+      <formula>3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G67">
     <cfRule type="cellIs" dxfId="49" priority="48" operator="greaterThan">
       <formula>"3.0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G66">
+  <conditionalFormatting sqref="G67">
     <cfRule type="cellIs" dxfId="48" priority="45" operator="equal">
       <formula>0</formula>
     </cfRule>
@@ -3945,7 +4192,7 @@
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G66">
+  <conditionalFormatting sqref="G67">
     <cfRule type="cellIs" dxfId="45" priority="43" operator="equal">
       <formula>"3.0"</formula>
     </cfRule>
@@ -3953,158 +4200,156 @@
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G14">
-    <cfRule type="cellIs" dxfId="43" priority="42" operator="greaterThan">
-      <formula>3</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G14">
-    <cfRule type="cellIs" dxfId="42" priority="39" operator="equal">
+  <conditionalFormatting sqref="G34">
+    <cfRule type="cellIs" dxfId="43" priority="34" operator="equal">
+      <formula>"3.0"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="42" priority="37" operator="greaterThan">
+      <formula>3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G34">
+    <cfRule type="cellIs" dxfId="41" priority="33" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="40" operator="between">
+    <cfRule type="cellIs" dxfId="40" priority="35" operator="between">
       <formula>"2.9"</formula>
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="41" operator="between">
+    <cfRule type="cellIs" dxfId="39" priority="36" operator="between">
       <formula>3</formula>
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G56">
-    <cfRule type="cellIs" dxfId="39" priority="38" operator="greaterThan">
-      <formula>"3.0"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G56">
-    <cfRule type="cellIs" dxfId="38" priority="35" operator="equal">
+  <conditionalFormatting sqref="F58">
+    <cfRule type="cellIs" dxfId="38" priority="31" operator="equal">
+      <formula>"3.0"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="37" priority="32" operator="greaterThan">
+      <formula>3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G58">
+    <cfRule type="cellIs" dxfId="36" priority="30" operator="greaterThan">
+      <formula>"3.0"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G58">
+    <cfRule type="cellIs" dxfId="35" priority="27" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="36" operator="between">
+    <cfRule type="cellIs" dxfId="34" priority="28" operator="between">
       <formula>"2.9"</formula>
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="37" operator="between">
+    <cfRule type="cellIs" dxfId="33" priority="29" operator="between">
       <formula>3</formula>
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G56">
-    <cfRule type="cellIs" dxfId="35" priority="33" operator="equal">
-      <formula>"3.0"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="34" operator="greaterThan">
-      <formula>3</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F67">
-    <cfRule type="cellIs" dxfId="33" priority="31" operator="equal">
-      <formula>"3.0"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="32" operator="greaterThan">
-      <formula>3</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G67">
-    <cfRule type="cellIs" dxfId="31" priority="30" operator="greaterThan">
-      <formula>"3.0"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G67">
-    <cfRule type="cellIs" dxfId="30" priority="27" operator="equal">
+  <conditionalFormatting sqref="G58">
+    <cfRule type="cellIs" dxfId="32" priority="25" operator="equal">
+      <formula>"3.0"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="31" priority="26" operator="greaterThan">
+      <formula>3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G31">
+    <cfRule type="cellIs" dxfId="30" priority="24" operator="greaterThan">
+      <formula>"3.0"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G31">
+    <cfRule type="cellIs" dxfId="29" priority="21" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="28" operator="between">
+    <cfRule type="cellIs" dxfId="28" priority="22" operator="between">
       <formula>"2.9"</formula>
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="29" operator="between">
+    <cfRule type="cellIs" dxfId="27" priority="23" operator="between">
       <formula>3</formula>
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G67">
-    <cfRule type="cellIs" dxfId="27" priority="25" operator="equal">
-      <formula>"3.0"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="26" operator="greaterThan">
-      <formula>3</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G34">
-    <cfRule type="cellIs" dxfId="25" priority="16" operator="equal">
-      <formula>"3.0"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="19" operator="greaterThan">
-      <formula>3</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G34">
-    <cfRule type="cellIs" dxfId="23" priority="15" operator="equal">
+  <conditionalFormatting sqref="F45">
+    <cfRule type="cellIs" dxfId="26" priority="19" operator="equal">
+      <formula>"3.0"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="25" priority="20" operator="greaterThan">
+      <formula>3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G66">
+    <cfRule type="cellIs" dxfId="17" priority="18" operator="greaterThan">
+      <formula>"3.0"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G66">
+    <cfRule type="cellIs" dxfId="14" priority="15" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="17" operator="between">
+    <cfRule type="cellIs" dxfId="15" priority="16" operator="between">
       <formula>"2.9"</formula>
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="18" operator="between">
+    <cfRule type="cellIs" dxfId="16" priority="17" operator="between">
       <formula>3</formula>
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F58">
-    <cfRule type="cellIs" dxfId="20" priority="13" operator="equal">
-      <formula>"3.0"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="14" operator="greaterThan">
-      <formula>3</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G58">
-    <cfRule type="cellIs" dxfId="18" priority="12" operator="greaterThan">
-      <formula>"3.0"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G58">
-    <cfRule type="cellIs" dxfId="17" priority="9" operator="equal">
+  <conditionalFormatting sqref="G66">
+    <cfRule type="cellIs" dxfId="13" priority="13" operator="equal">
+      <formula>"3.0"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="14" operator="greaterThan">
+      <formula>3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G40">
+    <cfRule type="cellIs" dxfId="11" priority="9" operator="equal">
+      <formula>"3.0"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="12" operator="greaterThan">
+      <formula>3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G40">
+    <cfRule type="cellIs" dxfId="9" priority="8" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="10" operator="between">
+    <cfRule type="cellIs" dxfId="8" priority="10" operator="between">
       <formula>"2.9"</formula>
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="11" operator="between">
+    <cfRule type="cellIs" dxfId="7" priority="11" operator="between">
       <formula>3</formula>
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G58">
-    <cfRule type="cellIs" dxfId="14" priority="7" operator="equal">
-      <formula>"3.0"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="8" operator="greaterThan">
-      <formula>3</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G31">
-    <cfRule type="cellIs" dxfId="12" priority="6" operator="greaterThan">
-      <formula>"3.0"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G31">
-    <cfRule type="cellIs" dxfId="11" priority="3" operator="equal">
+  <conditionalFormatting sqref="G36">
+    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
+      <formula>"3.0"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="7" operator="greaterThan">
+      <formula>3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G36">
+    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="4" operator="between">
+    <cfRule type="cellIs" dxfId="3" priority="5" operator="between">
       <formula>"2.9"</formula>
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="5" operator="between">
+    <cfRule type="cellIs" dxfId="2" priority="6" operator="between">
       <formula>3</formula>
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F45">
+  <conditionalFormatting sqref="F36">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"3.0"</formula>
     </cfRule>

</xml_diff>